<commit_message>
Added mask_bol feature, removed configurable
</commit_message>
<xml_diff>
--- a/data/G2 Port Code Mapping.xlsx
+++ b/data/G2 Port Code Mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tym.Teo\Documents\Delay Report - Rewrite\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D0C1CE-6D51-4AA1-AA90-806B5BBE8BA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45F05F97-4B82-403C-AFB7-08E8D2354A67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -114,14 +114,14 @@
     <t>Shanghai</t>
   </si>
   <si>
-    <t>G2 Port Name</t>
+    <t>Port Name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,12 +147,6 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFABB2BF"/>
-      <name val="Fira Code"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -190,19 +184,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -484,20 +475,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -505,7 +496,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -513,7 +504,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -521,7 +512,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -529,7 +520,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -537,107 +528,85 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="4"/>
-    </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E16" s="4"/>
-    </row>
-    <row r="17" spans="5:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="5:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="5:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E19" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>